<commit_message>
Complete EDA. This is good enough
</commit_message>
<xml_diff>
--- a/Excel_Challenge_529 - Sum with Signs.xlsx
+++ b/Excel_Challenge_529 - Sum with Signs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C21C6E8-3E8F-498B-989A-AB6C9AC4AA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A9CCF4-ACD5-4A36-A561-3D38F90867CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,11 +53,18 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1">
+  <futureMetadata name="XLRICHVALUE" count="2">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
         </ext>
       </extLst>
     </bk>
@@ -67,9 +74,12 @@
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1">
+  <valueMetadata count="2">
     <bk>
       <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -138,7 +148,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +167,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -170,11 +186,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,20 +439,29 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
   <rv s="0">
     <fb t="e">#N/A</fb>
     <v>6</v>
     <v>7</v>
   </rv>
+  <rv s="1">
+    <fb t="e">#N/A</fb>
+    <v>6</v>
+    <v>1</v>
+  </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
   <s t="_error">
     <k n="errorType" t="i"/>
     <k n="subType" t="i"/>
+  </s>
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="propagated" t="b"/>
   </s>
 </rvStructures>
 </file>
@@ -988,7 +1014,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C24"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1267,19 +1293,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF97E6D-3280-4E54-8FBE-3A89AB17265A}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.5546875" customWidth="1"/>
+    <col min="12" max="12" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1287,7 +1315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1301,8 +1329,21 @@
       <c r="D2" t="str">
         <v>340</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="4"/>
+      <c r="H2" cm="1">
+        <f t="array" ref="H2:I2">IF(IFERROR(FIND("-",_xlfn.ANCHORARRAY( C2)), 0), SUBSTITUTE(_xlfn.ANCHORARRAY(C2), "-", "") * -1,_xlfn.ANCHORARRAY( C2) + 0)</f>
+        <v>-98</v>
+      </c>
+      <c r="I2">
+        <v>340</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2">
+        <f>IFERROR(SUM(_xlfn.ANCHORARRAY(H2)),0)</f>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1319,8 +1360,24 @@
       <c r="E3" t="str">
         <v>629</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="4"/>
+      <c r="H3" cm="1">
+        <f t="array" ref="H3:J3">IF(IFERROR(FIND("-",_xlfn.ANCHORARRAY( C3)), 0), SUBSTITUTE(_xlfn.ANCHORARRAY(C3), "-", "") * -1,_xlfn.ANCHORARRAY( C3) + 0)</f>
+        <v>-785</v>
+      </c>
+      <c r="I3">
+        <v>-13</v>
+      </c>
+      <c r="J3">
+        <v>629</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3">
+        <f t="shared" ref="M3:M10" si="0">IFERROR(SUM(_xlfn.ANCHORARRAY(H3)),0)</f>
+        <v>-169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1340,8 +1397,27 @@
       <c r="F4" t="str">
         <v>-5218</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="4"/>
+      <c r="H4" cm="1">
+        <f t="array" ref="H4:K4">IF(IFERROR(FIND("-",_xlfn.ANCHORARRAY( C4)), 0), SUBSTITUTE(_xlfn.ANCHORARRAY(C4), "-", "") * -1,_xlfn.ANCHORARRAY( C4) + 0)</f>
+        <v>603</v>
+      </c>
+      <c r="I4">
+        <v>707</v>
+      </c>
+      <c r="J4">
+        <v>4086</v>
+      </c>
+      <c r="K4">
+        <v>-5218</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1352,8 +1428,18 @@
         <f t="array" ref="C5">_xlfn.REGEXEXTRACT(A5, "[0-9/-]+", 1)</f>
         <v>2647</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="4"/>
+      <c r="H5" cm="1">
+        <f t="array" ref="H5">IF(IFERROR(FIND("-",_xlfn.ANCHORARRAY( C5)), 0), SUBSTITUTE(_xlfn.ANCHORARRAY(C5), "-", "") * -1,_xlfn.ANCHORARRAY( C5) + 0)</f>
+        <v>2647</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>2647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1364,8 +1450,18 @@
         <f t="array" ref="C6">_xlfn.REGEXEXTRACT(A6, "[0-9/-]+", 1)</f>
         <v>456-</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="4"/>
+      <c r="H6" cm="1">
+        <f t="array" ref="H6">IF(IFERROR(FIND("-",_xlfn.ANCHORARRAY( C6)), 0), SUBSTITUTE(_xlfn.ANCHORARRAY(C6), "-", "") * -1,_xlfn.ANCHORARRAY( C6) + 0)</f>
+        <v>-456</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>-456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1376,8 +1472,18 @@
         <f t="array" ref="C7">_xlfn.REGEXEXTRACT(A7, "[0-9/-]+", 1)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="4"/>
+      <c r="H7" t="e" cm="1" vm="2">
+        <f t="array" ref="H7">IF(IFERROR(FIND("-",_xlfn.ANCHORARRAY( C7)), 0), SUBSTITUTE(_xlfn.ANCHORARRAY(C7), "-", "") * -1,_xlfn.ANCHORARRAY( C7) + 0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1397,8 +1503,27 @@
       <c r="F8" t="str">
         <v>233</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="4"/>
+      <c r="H8" cm="1">
+        <f t="array" ref="H8:K8">IF(IFERROR(FIND("-",_xlfn.ANCHORARRAY( C8)), 0), SUBSTITUTE(_xlfn.ANCHORARRAY(C8), "-", "") * -1,_xlfn.ANCHORARRAY( C8) + 0)</f>
+        <v>-98</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>-2</v>
+      </c>
+      <c r="K8">
+        <v>233</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1418,8 +1543,27 @@
       <c r="F9" t="str">
         <v>-4991</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="4"/>
+      <c r="H9" cm="1">
+        <f t="array" ref="H9:K9">IF(IFERROR(FIND("-",_xlfn.ANCHORARRAY( C9)), 0), SUBSTITUTE(_xlfn.ANCHORARRAY(C9), "-", "") * -1,_xlfn.ANCHORARRAY( C9) + 0)</f>
+        <v>4138</v>
+      </c>
+      <c r="I9">
+        <v>7371</v>
+      </c>
+      <c r="J9">
+        <v>7255</v>
+      </c>
+      <c r="K9">
+        <v>-4991</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>13773</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1438,6 +1582,25 @@
       </c>
       <c r="F10" t="str">
         <v>345-</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" cm="1">
+        <f t="array" ref="H10:K10">IF(IFERROR(FIND("-",_xlfn.ANCHORARRAY( C10)), 0), SUBSTITUTE(_xlfn.ANCHORARRAY(C10), "-", "") * -1,_xlfn.ANCHORARRAY( C10) + 0)</f>
+        <v>297</v>
+      </c>
+      <c r="I10">
+        <v>-297</v>
+      </c>
+      <c r="J10">
+        <v>345</v>
+      </c>
+      <c r="K10">
+        <v>-345</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>